<commit_message>
update file REST Coding Overview
</commit_message>
<xml_diff>
--- a/Knowledge/04_REST Coding_Overview_date.xlsx
+++ b/Knowledge/04_REST Coding_Overview_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SpringBootPrj\Knowledge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F443F3-D348-46DD-943F-1D49E161A53E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC7ED9F-C335-4765-81B1-4D3577B8F39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,119 +730,32 @@
     <t>Controller</t>
   </si>
   <si>
-    <r>
-      <t>Controller đ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ợc tạo để control request đ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ợc gửi tới server từ end user
-a. Các thuộc tính trong Controller: Repository (Xem #3)
-b. Các ph</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ươ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ng thức trong Controller: xử lý Post, xử lý Get, xử lý PUT, …
-**Các điểm cần l</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>u ý:
-Mỗi ph</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ươ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ng thức cần có annotation t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ươ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ng ứng</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    @GetMapping("/books/{id}")
+    <t>Tạo mới overview cho REST Coding</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public interface BookRepository extends JpaRepository&lt;Book, Long&gt; {} 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Book là 1 Entity class</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@RestController
+public class BookController {
+    @Autowired
+    private BookRepository repository;
+...
+    @GetMapping("/books/{id}")
     Book findOne(@PathVariable Long id){
         return repository.findById(id)
                 .orElseThrow(()-&gt;new BookNotFoundException(id));
@@ -851,6 +764,135 @@
   </si>
   <si>
     <r>
+      <t>Controller đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ợc tạo để control request đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ợc gửi tới server từ end user. Controller có annotation là @RestController
+a. Các thuộc tính trong Controller: Repository (Xem #3). Thuộc tính này đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ợc annotation bởi @Autowired
+b. Các ph</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ng thức trong Controller: xử lý Post, xử lý Get, xử lý PUT, …
+**Các điểm cần l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>u ý:
+Mỗi ph</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ng thức cần có annotation t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ng ứng</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
       <t>Repository Là n</t>
     </r>
     <r>
@@ -920,7 +962,7 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>ợc connect đến 1 database có sẵn 
+      <t>ợc connect đến 1 database có sẵn
 **Các điểm cần l</t>
     </r>
     <r>
@@ -939,29 +981,27 @@
         <charset val="128"/>
       </rPr>
       <t>u ý:
-JpaRepository&lt;T, Long&gt;, trong đó:
+1. JpaRepository&lt;T, Long&gt;, trong đó:
 T: tên entity
-Long: fixed, là id type</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Tạo mới overview cho REST Coding</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">public interface BookRepository extends JpaRepository&lt;Book, Long&gt; {} 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>Book là 1 Entity class</t>
+Long: fixed, là id type
+2. Ph</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ng thức khỏi tạo repository có annotation là @Bean</t>
     </r>
     <phoneticPr fontId="3"/>
   </si>
@@ -1776,6 +1816,27 @@
     <xf numFmtId="0" fontId="29" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1785,29 +1846,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2168,7 +2208,7 @@
         <v>44152</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>1</v>
@@ -2287,10 +2327,10 @@
       <c r="B2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="97"/>
+      <c r="D2" s="104"/>
       <c r="E2" s="36"/>
       <c r="F2" s="37"/>
     </row>
@@ -2301,10 +2341,10 @@
       <c r="B3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="99"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="36"/>
       <c r="F3" s="37"/>
     </row>
@@ -2315,10 +2355,10 @@
       <c r="B4" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="99"/>
+      <c r="D4" s="106"/>
       <c r="E4" s="36"/>
       <c r="F4" s="37"/>
     </row>
@@ -2329,10 +2369,10 @@
       <c r="B5" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="100"/>
+      <c r="D5" s="101"/>
       <c r="E5" s="36"/>
       <c r="F5" s="42"/>
     </row>
@@ -2343,18 +2383,18 @@
       <c r="B6" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="100"/>
+      <c r="D6" s="101"/>
       <c r="E6" s="36"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104">
+      <c r="A7" s="102">
         <v>6</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="100" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="44" t="s">
@@ -2367,8 +2407,8 @@
       <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="105"/>
-      <c r="B8" s="102"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="46" t="s">
         <v>49</v>
       </c>
@@ -2379,8 +2419,8 @@
       <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="105"/>
-      <c r="B9" s="102"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="99"/>
       <c r="C9" s="46" t="s">
         <v>50</v>
       </c>
@@ -2391,8 +2431,8 @@
       <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="105"/>
-      <c r="B10" s="102"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="48" t="s">
         <v>51</v>
       </c>
@@ -2403,8 +2443,8 @@
       <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="105"/>
-      <c r="B11" s="102"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="49" t="s">
         <v>52</v>
       </c>
@@ -2421,10 +2461,10 @@
       <c r="B12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="98" t="s">
+      <c r="C12" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="99"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="36"/>
       <c r="F12" s="37"/>
     </row>
@@ -2435,10 +2475,10 @@
       <c r="B13" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="99"/>
+      <c r="D13" s="106"/>
       <c r="E13" s="36"/>
       <c r="F13" s="37"/>
     </row>
@@ -2540,17 +2580,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2647,11 +2687,11 @@
       <c r="G5" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="106" t="s">
+      <c r="H5" s="97" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="96" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="120" x14ac:dyDescent="0.4">
       <c r="B6" s="75">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2665,10 +2705,10 @@
       </c>
       <c r="F6" s="78"/>
       <c r="G6" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="107" t="s">
         <v>74</v>
+      </c>
+      <c r="H6" s="98" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="101.25" x14ac:dyDescent="0.4">
@@ -2687,11 +2727,11 @@
       <c r="G7" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="107" t="s">
+      <c r="H7" s="98" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="84" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="123.75" x14ac:dyDescent="0.4">
       <c r="B8" s="75">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2705,10 +2745,10 @@
       </c>
       <c r="F8" s="78"/>
       <c r="G8" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="107" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="H8" s="97" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">

</xml_diff>